<commit_message>
remove one term excluded from generation
</commit_message>
<xml_diff>
--- a/doc/Ontorat/assay/20141202_OBI_assay_output.xlsx
+++ b/doc/Ontorat/assay/20141202_OBI_assay_output.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="510" yWindow="540" windowWidth="20775" windowHeight="11190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
   <si>
     <t>Term ID</t>
   </si>
@@ -291,93 +290,54 @@
   </si>
   <si>
     <t>An assay that identifies epigenetic modification including histone modifications, open chromatin, and DNA methylation.</t>
-  </si>
-  <si>
-    <t>OBI_0002021</t>
-  </si>
-  <si>
-    <t>transcription factor binding site identification assay</t>
-  </si>
-  <si>
-    <t>TF Binding</t>
-  </si>
-  <si>
-    <t>An assay that identifies where a transcription factor binds specifically on a nucleic acid.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="11"/>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="11"/>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="single"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <sz val="10"/>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <sz val="10"/>
-      <b val="1"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="10"/>
-      <b val="1"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <sz val="11"/>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="single"/>
-      <strike val="0"/>
-      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="none">
@@ -387,51 +347,44 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -719,55 +672,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:AL11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="58.7109375" customWidth="true" style="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="true" style="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="true" style="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="true" style="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="true" style="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="true" style="1"/>
-    <col min="8" max="8" width="98" customWidth="true" style="2"/>
-    <col min="9" max="9" width="31.140625" customWidth="true" style="1"/>
-    <col min="10" max="10" width="29.5703125" customWidth="true" style="1"/>
-    <col min="11" max="11" width="47.140625" customWidth="true" style="1"/>
-    <col min="12" max="12" width="14" customWidth="true" style="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="true" style="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="true" style="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="true" style="1"/>
-    <col min="16" max="16" width="13.42578125" customWidth="true" style="1"/>
-    <col min="17" max="17" width="17.7109375" customWidth="true" style="1"/>
-    <col min="18" max="18" width="15.42578125" customWidth="true" style="1"/>
-    <col min="19" max="19" width="15.5703125" customWidth="true" style="1"/>
-    <col min="20" max="20" width="14.7109375" customWidth="true" style="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="true" style="1"/>
-    <col min="22" max="22" width="9.140625" customWidth="true" style="1"/>
-    <col min="23" max="23" width="9.140625" customWidth="true" style="1"/>
-    <col min="24" max="24" width="9.140625" customWidth="true" style="1"/>
-    <col min="25" max="25" width="9.140625" customWidth="true" style="1"/>
-    <col min="26" max="26" width="9.140625" customWidth="true" style="1"/>
-    <col min="27" max="27" width="9.140625" customWidth="true" style="1"/>
-    <col min="28" max="28" width="9.140625" customWidth="true" style="1"/>
-    <col min="29" max="29" width="14.5703125" customWidth="true" style="1"/>
-    <col min="30" max="30" width="12.85546875" customWidth="true" style="1"/>
-    <col min="31" max="31" width="9.140625" customWidth="true" style="1"/>
-    <col min="32" max="32" width="15.28515625" customWidth="true" style="1"/>
-    <col min="33" max="33" width="28.85546875" customWidth="true" style="1"/>
-    <col min="34" max="34" width="14.5703125" customWidth="true" style="1"/>
-    <col min="35" max="35" width="31.140625" customWidth="true" style="1"/>
-    <col min="36" max="36" width="42.42578125" customWidth="true" style="1"/>
-    <col min="37" max="37" width="9.140625" customWidth="true" style="1"/>
+    <col min="2" max="2" width="58.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="98" style="2" customWidth="1"/>
+    <col min="9" max="9" width="31.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="47.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" style="1" customWidth="1"/>
+    <col min="21" max="28" width="9.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5703125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.85546875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="15.28515625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="28.85546875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="14.5703125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="31.140625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="42.42578125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" customHeight="1" ht="17.25" s="9" customFormat="1">
+    <row r="1" spans="1:38" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -877,7 +822,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -940,10 +885,9 @@
       <c r="AJ2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AK2" t="s"/>
-      <c r="AL2" t="s"/>
+      <c r="AK2"/>
     </row>
-    <row r="3" spans="1:38" customHeight="1" ht="15">
+    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1018,10 +962,9 @@
       <c r="AJ3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AK3" t="s"/>
-      <c r="AL3" t="s"/>
+      <c r="AK3"/>
     </row>
-    <row r="4" spans="1:38" customHeight="1" ht="15">
+    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1084,10 +1027,9 @@
       <c r="AJ4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AK4" t="s"/>
-      <c r="AL4" t="s"/>
+      <c r="AK4"/>
     </row>
-    <row r="5" spans="1:38" customHeight="1" ht="15.75">
+    <row r="5" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -1150,10 +1092,9 @@
       <c r="AJ5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AK5" t="s"/>
-      <c r="AL5" t="s"/>
+      <c r="AK5"/>
     </row>
-    <row r="6" spans="1:38" customHeight="1" ht="15">
+    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1216,10 +1157,9 @@
       <c r="AJ6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AK6" t="s"/>
-      <c r="AL6" t="s"/>
+      <c r="AK6"/>
     </row>
-    <row r="7" spans="1:38" customHeight="1" ht="15">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -1282,10 +1222,9 @@
       <c r="AJ7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AK7" t="s"/>
-      <c r="AL7" t="s"/>
+      <c r="AK7"/>
     </row>
-    <row r="8" spans="1:38" customHeight="1" ht="17.25" s="9" customFormat="1">
+    <row r="8" spans="1:38" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -1342,170 +1281,91 @@
       <c r="AJ8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AK8" t="s"/>
-      <c r="AL8" t="s"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
     </row>
-    <row r="9" spans="1:38" customHeight="1" ht="17.25" s="9" customFormat="1">
-      <c r="A9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH9" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK9" t="s"/>
-      <c r="AL9" t="s"/>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9" s="3"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AK9"/>
     </row>
-    <row r="10" spans="1:38">
-      <c r="A10" t="s"/>
-      <c r="B10" t="s"/>
-      <c r="C10" t="s"/>
-      <c r="D10" t="s"/>
-      <c r="E10" t="s"/>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
       <c r="F10"/>
-      <c r="G10" s="3"/>
-      <c r="H10" t="s"/>
-      <c r="I10" t="s"/>
-      <c r="J10" t="s"/>
-      <c r="K10" t="s"/>
-      <c r="L10" t="s"/>
-      <c r="M10" t="s"/>
-      <c r="N10" t="s"/>
-      <c r="O10" t="s"/>
-      <c r="P10" t="s"/>
-      <c r="Q10" t="s"/>
-      <c r="R10" t="s"/>
-      <c r="S10" t="s"/>
-      <c r="T10" t="s"/>
-      <c r="U10" t="s"/>
-      <c r="V10" t="s"/>
-      <c r="W10" t="s"/>
-      <c r="X10" t="s"/>
-      <c r="Y10" t="s"/>
-      <c r="Z10" t="s"/>
-      <c r="AA10" t="s"/>
-      <c r="AB10" t="s"/>
-      <c r="AC10" t="s"/>
-      <c r="AD10" t="s"/>
-      <c r="AE10" t="s"/>
-      <c r="AF10" t="s"/>
-      <c r="AG10" t="s"/>
-      <c r="AH10" t="s"/>
-      <c r="AI10" t="s"/>
-      <c r="AJ10" t="s"/>
-      <c r="AK10" t="s"/>
-      <c r="AL10" t="s"/>
-    </row>
-    <row r="11" spans="1:38">
-      <c r="A11" t="s"/>
-      <c r="B11" t="s"/>
-      <c r="C11" t="s"/>
-      <c r="D11" t="s"/>
-      <c r="E11" t="s"/>
-      <c r="F11" t="s"/>
-      <c r="G11" t="s"/>
-      <c r="H11"/>
-      <c r="I11" s="2"/>
-      <c r="J11" t="s"/>
-      <c r="K11" t="s"/>
-      <c r="L11" t="s"/>
-      <c r="M11" t="s"/>
-      <c r="N11" t="s"/>
-      <c r="O11" t="s"/>
-      <c r="P11" t="s"/>
-      <c r="Q11" t="s"/>
-      <c r="R11" t="s"/>
-      <c r="S11" t="s"/>
-      <c r="T11" t="s"/>
-      <c r="U11" t="s"/>
-      <c r="V11" t="s"/>
-      <c r="W11" t="s"/>
-      <c r="X11" t="s"/>
-      <c r="Y11" t="s"/>
-      <c r="Z11" t="s"/>
-      <c r="AA11" t="s"/>
-      <c r="AB11" t="s"/>
-      <c r="AC11" t="s"/>
-      <c r="AD11" t="s"/>
-      <c r="AE11" t="s"/>
-      <c r="AF11" t="s"/>
-      <c r="AG11" t="s"/>
-      <c r="AH11" t="s"/>
-      <c r="AI11" t="s"/>
-      <c r="AJ11" t="s"/>
-      <c r="AK11" t="s"/>
-      <c r="AL11" t="s"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10" s="2"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AK10"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId_hyperlink_1"/>
+    <hyperlink ref="I3" r:id="rId1"/>
   </hyperlinks>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>